<commit_message>
Documentación del proyecto actualización
</commit_message>
<xml_diff>
--- a/Documentación/Planeación.xlsx
+++ b/Documentación/Planeación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/313df3f7be5e54e9/Documentos/Mastr/Ing. Software/Proyecto final Semestre I/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/313df3f7be5e54e9/Documentos/Mastr/Ing. Software/SW/project/Documentación/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="452" documentId="8_{34A46EF9-AC0D-4218-985F-0FD8493F8371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6262F6E-0B37-45E6-A3AB-CE39D15A992B}"/>
@@ -1692,7 +1692,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>